<commit_message>
[fix][cloudkitty] Add code for optimized to rating download xlsx eg.
</commit_message>
<xml_diff>
--- a/dingo_command/api/template/rating_summary_template.xlsx
+++ b/dingo_command/api/template/rating_summary_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6880" firstSheet="1"/>
+    <workbookView windowHeight="17655" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="ratingSummary" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Begin</t>
+    <t>Begin(Timezone: UTC)</t>
   </si>
   <si>
-    <t>End</t>
+    <t>End(Timezone: UTC)</t>
   </si>
   <si>
     <t>Project ID</t>
@@ -1038,13 +1038,13 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D$1:D$1048576"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.6666666666667" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.5833333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="34.5833333333333" style="2" customWidth="1"/>
     <col min="4" max="4" width="91.0833333333333" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
[fix][cloudkitty] remove filtering and projectId columns
</commit_message>
<xml_diff>
--- a/dingo_command/api/template/rating_summary_template.xlsx
+++ b/dingo_command/api/template/rating_summary_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17655" firstSheet="1"/>
+    <workbookView windowWidth="28800" windowHeight="12255" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="ratingSummary" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Begin(Timezone: UTC)</t>
+    <t>Begin</t>
   </si>
   <si>
-    <t>End(Timezone: UTC)</t>
-  </si>
-  <si>
-    <t>Project ID</t>
+    <t>End</t>
   </si>
   <si>
     <t>Resources</t>
@@ -1033,24 +1030,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="25.125" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.5833333333333" style="2" customWidth="1"/>
-    <col min="4" max="4" width="91.0833333333333" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1" customWidth="1"/>
+    <col min="3" max="3" width="91.0833333333333" style="2" customWidth="1"/>
+    <col min="4" max="16383" width="9" style="1" customWidth="1"/>
+    <col min="16384" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:13">
+    <row r="1" ht="15.75" customHeight="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1060,378 +1057,314 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="17" s="1" customFormat="1" spans="1:3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="25" s="1" customFormat="1" spans="1:3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="26" s="1" customFormat="1" spans="1:3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="28" s="1" customFormat="1" spans="1:3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="29" s="1" customFormat="1" spans="1:3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="30" s="1" customFormat="1" spans="1:3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="32" s="1" customFormat="1" spans="1:3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="33" s="1" customFormat="1" spans="1:3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="34" s="1" customFormat="1" spans="1:3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="35" s="1" customFormat="1" spans="1:3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="36" s="1" customFormat="1" spans="1:3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="37" s="1" customFormat="1" spans="1:3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="38" s="1" customFormat="1" spans="1:3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="39" s="1" customFormat="1" spans="1:3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="40" s="1" customFormat="1" spans="1:3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="41" s="1" customFormat="1" spans="1:3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="42" s="1" customFormat="1" spans="1:3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="43" s="1" customFormat="1" spans="1:3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="44" s="1" customFormat="1" spans="1:3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="45" s="1" customFormat="1" spans="1:3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="46" s="1" customFormat="1" spans="1:3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="47" s="1" customFormat="1" spans="1:3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="48" s="1" customFormat="1" spans="1:3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="49" s="1" customFormat="1" spans="1:3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="50" s="1" customFormat="1" spans="1:3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="51" s="1" customFormat="1" spans="1:3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="58" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="58" s="1" customFormat="1" spans="1:3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="59" s="1" customFormat="1" spans="1:3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="60" s="1" customFormat="1" spans="1:3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="61" s="1" customFormat="1" spans="1:3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="63" s="1" customFormat="1" spans="1:3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="64" s="1" customFormat="1" spans="1:3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="65" s="1" customFormat="1" spans="1:3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="66" s="1" customFormat="1" spans="1:3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="67" s="1" customFormat="1" spans="1:3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" s="1" customFormat="1" spans="1:4">
+    </row>
+    <row r="68" s="1" customFormat="1" spans="1:3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>